<commit_message>
beta & cost of equity
</commit_message>
<xml_diff>
--- a/bvb weekly price action.xlsx
+++ b/bvb weekly price action.xlsx
@@ -9692,4 +9692,10 @@
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.75"/>
   <pageSetup fitToHeight="0"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{ea60d57e-af5b-4752-ac57-3e4f28ca11dc}" enabled="1" method="Standard" siteId="{36da45f1-dd2c-4d1f-af13-5abe46b99921}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>